<commit_message>
Atualização automática: 2025-08-07 11:01:17
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1133,6 +1133,98 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>312b9e21-1bbf-4ba0-ad02-ea0aaa6f842b</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mosca</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>45876</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>image_20250807111026_ppp0.jpg</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>PLACA_20250717165933</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Beja</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>38.02035</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-7.94715</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>641,529,688,576</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>0.75</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>d46143c3-a87f-42fc-a10d-2d5a22dc0c2b</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mosca</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>45876</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>image_20250807111026_ppp0.jpg</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>PLACA_20250717165933</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Beja</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>38.02035</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-7.94715</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>793,481,831,526</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-08 10:00:35
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1225,6 +1225,52 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ce49ea82-267b-4cc5-86c9-7e4337c56079</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mosca</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>45877</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>image_20250808100711_ppp0.jpg</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>PLACA_20250717165933</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Beja</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>38.02035</v>
+      </c>
+      <c r="H18" t="n">
+        <v>-7.94715</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>1182,409,1232,451</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0.75</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-08 22:00:24
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111026_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>641,529,688,576</t>
+          <t>643,531,686,575</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111026_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>793,481,831,526</t>
+          <t>794,481,830,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
@@ -1266,6 +1266,52 @@
         </is>
       </c>
       <c r="J18" t="inlineStr">
+        <is>
+          <t>0.75</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>f77cad75-e373-4760-9d5a-1d927bfccd1d</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mosca</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>45877</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>image_20250808221835_ppp0.jpg</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>PLACA_20250717165933</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Beja</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>38.02035</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-7.94715</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>819,160,858,215</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
         <is>
           <t>0.75</t>
         </is>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-09 09:00:53
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>643,531,686,575</t>
+          <t>641,530,687,575</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,830,526</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-09 21:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>735a78bc-70c4-49a0-8b97-230d0c9db5e1</t>
+          <t>44912068-946a-41df-b25e-ddfc1b484d3c</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>44912068-946a-41df-b25e-ddfc1b484d3c</t>
+          <t>a0d98e9c-5504-42a7-9e55-90c1f5f918d2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a0d98e9c-5504-42a7-9e55-90c1f5f918d2</t>
+          <t>3ce7cd97-85b1-4257-97de-19570753854d</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3ce7cd97-85b1-4257-97de-19570753854d</t>
+          <t>50759eb2-c2f5-4e05-88a0-868809c7749e</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>50759eb2-c2f5-4e05-88a0-868809c7749e</t>
+          <t>735a78bc-70c4-49a0-8b97-230d0c9db5e1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>641,530,687,575</t>
+          <t>642,530,686,576</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-08-10 09:00:44
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>44912068-946a-41df-b25e-ddfc1b484d3c</t>
+          <t>735a78bc-70c4-49a0-8b97-230d0c9db5e1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a0d98e9c-5504-42a7-9e55-90c1f5f918d2</t>
+          <t>44912068-946a-41df-b25e-ddfc1b484d3c</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3ce7cd97-85b1-4257-97de-19570753854d</t>
+          <t>a0d98e9c-5504-42a7-9e55-90c1f5f918d2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>50759eb2-c2f5-4e05-88a0-868809c7749e</t>
+          <t>3ce7cd97-85b1-4257-97de-19570753854d</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>735a78bc-70c4-49a0-8b97-230d0c9db5e1</t>
+          <t>50759eb2-c2f5-4e05-88a0-868809c7749e</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-10 21:00:24
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-11 08:49:38
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>735a78bc-70c4-49a0-8b97-230d0c9db5e1</t>
+          <t>44912068-946a-41df-b25e-ddfc1b484d3c</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>44912068-946a-41df-b25e-ddfc1b484d3c</t>
+          <t>a0d98e9c-5504-42a7-9e55-90c1f5f918d2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a0d98e9c-5504-42a7-9e55-90c1f5f918d2</t>
+          <t>3ce7cd97-85b1-4257-97de-19570753854d</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3ce7cd97-85b1-4257-97de-19570753854d</t>
+          <t>50759eb2-c2f5-4e05-88a0-868809c7749e</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>50759eb2-c2f5-4e05-88a0-868809c7749e</t>
+          <t>735a78bc-70c4-49a0-8b97-230d0c9db5e1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-12 09:01:14
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>642,530,686,574</t>
+          <t>641,530,687,575</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-12 21:00:24
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807110716_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>641,530,687,575</t>
+          <t>641,530,686,576</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807110716_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-08-13 09:00:24
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807110716_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>641,530,686,576</t>
+          <t>642,530,686,576</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807110716_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-08-13 21:00:24
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>642,530,686,576</t>
+          <t>642,530,686,574</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-14 09:00:55
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111026_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>642,530,686,574</t>
+          <t>641,529,688,576</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111026_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>793,481,831,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-14 21:00:24
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111026_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>641,529,688,576</t>
+          <t>642,530,686,576</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111026_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>793,481,831,526</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-15 09:00:24
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>642,530,686,576</t>
+          <t>641,530,687,575</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-15 21:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>641,530,687,575</t>
+          <t>643,531,686,575</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,830,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-16 21:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-17 09:01:04
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807110716_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>643,531,686,575</t>
+          <t>641,530,686,576</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807110716_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,830,526</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-17 21:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807110716_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>641,530,686,576</t>
+          <t>642,530,686,576</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807110716_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-08-18 09:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807111026_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>642,530,686,576</t>
+          <t>641,529,688,576</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807111026_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>793,481,831,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-18 21:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111026_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>641,529,688,576</t>
+          <t>642,530,686,574</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111026_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>793,481,831,526</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-08-19 09:01:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-19 21:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>642,530,686,574</t>
+          <t>643,531,686,575</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>794,481,830,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-20 09:01:05
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-21 09:01:14
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>643,531,686,575</t>
+          <t>641,530,687,575</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,830,526</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-21 21:00:24
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-22 21:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1317,6 +1317,52 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>89ec9c17-dac0-435a-851d-754b073844e5</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mosca</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>45891</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>image_20250822211929_ppp0.jpg</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>PLACA_20250717165933</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Beja</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>38.02035</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-7.94715</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>1022,1004,1060,1059</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>0.68</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-23 09:00:53
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>641,530,687,575</t>
+          <t>643,531,686,575</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,830,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-23 21:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>643,531,686,575</t>
+          <t>642,530,686,576</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,830,526</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-24 09:00:44
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>642,530,686,576</t>
+          <t>642,530,686,574</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>
@@ -1360,6 +1360,52 @@
       <c r="J20" t="inlineStr">
         <is>
           <t>0.68</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>a2ea21b8-7dce-4e6a-be35-4edaddca5896</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mosca</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>45893</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>image_20250824092407_ppp0.jpg</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>PLACA_20250717165933</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Beja</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>38.02035</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-7.94715</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>1002,789,1039,825</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>0.64</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-24 21:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>642,530,686,574</t>
+          <t>642,530,686,576</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>
@@ -1406,6 +1406,52 @@
       <c r="J21" t="inlineStr">
         <is>
           <t>0.64</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>66efa766-1456-4beb-b92a-0615a2fc41bb</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mosca</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>45893</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>image_20250824214658_ppp0.jpg</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>PLACA_20250717165933</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Beja</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>38.02035</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-7.94715</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>1272,293,1315,331</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>0.69</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-25 09:01:24
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>642,530,686,576</t>
+          <t>642,530,686,574</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-25 21:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>642,530,686,574</t>
+          <t>643,531,686,575</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>794,481,830,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-26 09:00:46
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807111026_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>643,531,686,575</t>
+          <t>641,529,688,576</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807111026_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,830,526</t>
+          <t>793,481,831,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1366,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>a2ea21b8-7dce-4e6a-be35-4edaddca5896</t>
+          <t>66efa766-1456-4beb-b92a-0615a2fc41bb</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>image_20250824092407_ppp0.jpg</t>
+          <t>image_20250824214658_ppp0.jpg</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1400,19 +1400,19 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>1002,789,1039,825</t>
+          <t>1272,293,1315,331</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>0.64</t>
+          <t>0.69</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>66efa766-1456-4beb-b92a-0615a2fc41bb</t>
+          <t>a2ea21b8-7dce-4e6a-be35-4edaddca5896</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1446,12 +1446,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>1272,293,1315,331</t>
+          <t>999,782,1040,825</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0.69</t>
+          <t>0.58</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-26 21:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111026_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>641,529,688,576</t>
+          <t>641,530,687,575</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111026_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>793,481,831,526</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-27 09:00:35
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>641,530,687,575</t>
+          <t>642,530,686,574</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-27 21:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>642,530,686,574</t>
+          <t>642,530,686,576</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-28 09:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>642,530,686,576</t>
+          <t>643,531,686,575</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>794,481,830,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-28 21:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>643,531,686,575</t>
+          <t>642,530,686,574</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,830,526</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-29 09:00:45
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1366,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>66efa766-1456-4beb-b92a-0615a2fc41bb</t>
+          <t>a2ea21b8-7dce-4e6a-be35-4edaddca5896</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>image_20250824214658_ppp0.jpg</t>
+          <t>image_20250824092407_ppp0.jpg</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1400,19 +1400,19 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>1272,293,1315,331</t>
+          <t>1002,789,1039,825</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>0.69</t>
+          <t>0.64</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>a2ea21b8-7dce-4e6a-be35-4edaddca5896</t>
+          <t>66efa766-1456-4beb-b92a-0615a2fc41bb</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1446,12 +1446,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>999,782,1040,825</t>
+          <t>1272,293,1315,331</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0.58</t>
+          <t>0.69</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-29 21:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1366,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>a2ea21b8-7dce-4e6a-be35-4edaddca5896</t>
+          <t>66efa766-1456-4beb-b92a-0615a2fc41bb</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>image_20250824092407_ppp0.jpg</t>
+          <t>image_20250824214658_ppp0.jpg</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1400,19 +1400,19 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>1002,789,1039,825</t>
+          <t>1272,293,1315,331</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>0.64</t>
+          <t>0.69</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>66efa766-1456-4beb-b92a-0615a2fc41bb</t>
+          <t>a2ea21b8-7dce-4e6a-be35-4edaddca5896</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1446,12 +1446,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>1272,293,1315,331</t>
+          <t>999,782,1040,825</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0.69</t>
+          <t>0.58</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-30 09:01:04
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111026_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>642,530,686,574</t>
+          <t>641,529,688,576</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111026_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>793,481,831,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-08-30 21:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250807111026_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>641,529,688,576</t>
+          <t>643,531,686,575</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>image_20250807111026_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>793,481,831,526</t>
+          <t>794,481,830,526</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-31 09:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-08-31 21:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>
@@ -1452,6 +1452,52 @@
       <c r="J22" t="inlineStr">
         <is>
           <t>0.58</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>00deb925-04cf-4a0c-b2a2-5289a118de4d</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>mosca</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>45900</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>image_20250831214359_ppp0.jpg</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>PLACA_20250717165933</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Beja</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>38.02035</v>
+      </c>
+      <c r="H23" t="n">
+        <v>-7.94715</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>1256,526,1294,578</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>0.72</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-01 09:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1366,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>66efa766-1456-4beb-b92a-0615a2fc41bb</t>
+          <t>a2ea21b8-7dce-4e6a-be35-4edaddca5896</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>image_20250824214658_ppp0.jpg</t>
+          <t>image_20250824092407_ppp0.jpg</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1400,19 +1400,19 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>1272,293,1315,331</t>
+          <t>1002,789,1039,825</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>0.69</t>
+          <t>0.64</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>a2ea21b8-7dce-4e6a-be35-4edaddca5896</t>
+          <t>66efa766-1456-4beb-b92a-0615a2fc41bb</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1446,12 +1446,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>999,782,1040,825</t>
+          <t>1272,293,1315,331</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0.58</t>
+          <t>0.69</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-01 21:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1366,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>a2ea21b8-7dce-4e6a-be35-4edaddca5896</t>
+          <t>66efa766-1456-4beb-b92a-0615a2fc41bb</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>image_20250824092407_ppp0.jpg</t>
+          <t>image_20250824214658_ppp0.jpg</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1400,19 +1400,19 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>1002,789,1039,825</t>
+          <t>1272,293,1315,331</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>0.64</t>
+          <t>0.69</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>66efa766-1456-4beb-b92a-0615a2fc41bb</t>
+          <t>a2ea21b8-7dce-4e6a-be35-4edaddca5896</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1446,12 +1446,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>1272,293,1315,331</t>
+          <t>999,782,1040,825</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0.69</t>
+          <t>0.58</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-02 09:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
@@ -1498,6 +1498,52 @@
       <c r="J23" t="inlineStr">
         <is>
           <t>0.72</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>687a4eaa-64d4-4e21-a791-c5a0b5673343</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>mosca</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>45902</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>image_20250902091301_ppp0.jpg</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>PLACA_20250717165933</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Beja</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>38.02035</v>
+      </c>
+      <c r="H24" t="n">
+        <v>-7.94715</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>1,0,703,1072</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>0.66</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-02 21:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1262,12 +1262,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-04 09:00:46
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-04 21:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-05 09:00:25
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
+          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,40 +735,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>image_20250728214139_ppp0.jpg</t>
+          <t>image_20250727074723_ppp0.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PLACA_20250717165933</t>
+          <t>PLACA_20250723145134</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Beja</t>
+          <t>Moura</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>38.02035</v>
+        <v>38.06587</v>
       </c>
       <c r="H7" t="n">
-        <v>-7.94715</v>
+        <v>-7.221796</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>962,713,1006,765</t>
+          <t>1490,161,1563,258</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
+          <t>283b6eda-9c83-4cdd-9524-c7c394f2dc89</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -802,19 +802,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>967,614,1002,659</t>
+          <t>962,713,1006,765</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
+          <t>a19b65d1-6f97-4841-9e1c-7446a9be92b6</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -848,19 +848,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>702,633,740,690</t>
+          <t>967,614,1002,659</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.73</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
+          <t>4be1b1cf-d480-453e-b5fb-d4ecd6764c4d</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,19 +894,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1254,850,1294,895</t>
+          <t>702,633,740,690</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.67</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2117575c-4ae1-458c-b88a-fc40f40debdb</t>
+          <t>dfd476d4-7689-4671-a076-78fe3ce806bb</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -919,33 +919,33 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>image_20250727074723_ppp0.jpg</t>
+          <t>image_20250728214139_ppp0.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLACA_20250723145134</t>
+          <t>PLACA_20250717165933</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Moura</t>
+          <t>Beja</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>38.06587</v>
+        <v>38.02035</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.221796</v>
+        <v>-7.94715</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1490,161,1563,258</t>
+          <t>1254,850,1294,895</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.67</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-05 10:30:17
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -492,7 +492,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>c0216a7d-c399-47cc-a93a-5cf8582753af</t>
+          <t>77ab58b0-f669-4e6e-b26e-a8357789d080</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -538,7 +538,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>58f80a35-44d8-4e2f-88e3-056ab899d16f</t>
+          <t>a2ec7b01-97e7-4b31-af0a-22843e0d5bee</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -584,7 +584,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>bafa3dd4-9e0d-4570-a592-47d8a622407a</t>
+          <t>7052c8df-2109-410c-abdc-73e3daa3ba50</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -630,7 +630,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>e0533abd-5a99-4617-9f36-d58682da62ea</t>
+          <t>e2cbd333-6275-4a76-bbad-aa32bea23534</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>76498aff-a520-434f-94db-490babc98cc6</t>
+          <t>543110a9-c7fb-4592-a759-ecd8bde4dc23</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>b6fa6e1b-2212-4233-946b-ef9a27ff5d1a</t>
+          <t>42ef002b-b4ac-40f9-910b-b83fc5bb7ef5</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -768,7 +768,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>721a3533-e61f-4b93-9ff6-f5d65a10e759</t>
+          <t>41477a7c-27ad-4394-b514-bc99c3388894</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -814,7 +814,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3332d274-226a-4abd-9c7a-ca90000ce5c8</t>
+          <t>54832180-8534-4b92-9a57-4176f97aacfa</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -860,7 +860,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9a39fa7b-4946-4a53-9e70-a178c93e5036</t>
+          <t>6c9080bb-8061-4711-b02a-7da01338beb8</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -906,7 +906,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>b9ebaf66-a976-4982-b88a-1a9a928cdc0a</t>
+          <t>c45d0f6d-e5c1-4d33-94f5-2e886b60bf19</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -952,7 +952,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2d26cd27-2383-4d14-b973-4cfd9392ce47</t>
+          <t>10ffe120-07be-4ac0-a3ee-2417c74c09ad</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>7420e0bb-0427-4925-8122-93388c4441f4</t>
+          <t>4c42a4de-c483-4b00-9621-9bbfd1c3a6e5</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1044,7 +1044,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ce39d27a-e73d-4336-b6f9-08aa6ebbb68d</t>
+          <t>4e2f94bd-6e7f-47c6-99ad-48b96ff1a18b</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1090,7 +1090,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>07c4c8b4-c2ed-4ef5-b379-f782e21c12bc</t>
+          <t>f5e1e006-f68b-4a12-a7ea-10f71a9f73a6</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1136,7 +1136,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>663fab28-83d3-405d-aa08-a0ac1d615dea</t>
+          <t>40c98c1d-9f79-456e-ae83-a5703fa69e74</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1182,7 +1182,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>565043c3-4934-4687-941f-2b510fa0b13a</t>
+          <t>da62cb63-8bf7-4b28-8536-bfa48dcdebb7</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1228,7 +1228,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>7f60d8cd-f991-4147-a41e-fcc3547caf80</t>
+          <t>78469df7-4600-4f34-a464-3abf5b3946b9</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1274,7 +1274,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>b173ae2d-fd7c-4cd6-b255-668fe1ef72bd</t>
+          <t>dd901bee-2756-43e2-b2b0-0dfca5c04baa</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-09-05 11:00:10
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -492,7 +492,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>77ab58b0-f669-4e6e-b26e-a8357789d080</t>
+          <t>320891a7-9716-4af5-a792-4bc855814887</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -538,7 +538,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>a2ec7b01-97e7-4b31-af0a-22843e0d5bee</t>
+          <t>cf5b1d2d-e6a6-4890-86b7-727104c438c7</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -584,7 +584,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>7052c8df-2109-410c-abdc-73e3daa3ba50</t>
+          <t>d3e26aa8-f8ad-4659-9e10-e2504a577d64</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -630,7 +630,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>e2cbd333-6275-4a76-bbad-aa32bea23534</t>
+          <t>4b7d1a0a-7be9-4095-8d08-3fe1aa818667</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>543110a9-c7fb-4592-a759-ecd8bde4dc23</t>
+          <t>2cdb1266-8286-4b3d-9247-3002269e62d9</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>42ef002b-b4ac-40f9-910b-b83fc5bb7ef5</t>
+          <t>64c4f383-9171-430f-bdb5-9a39599a9a14</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -768,7 +768,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>41477a7c-27ad-4394-b514-bc99c3388894</t>
+          <t>1cccb561-3eb4-4319-b0e2-f02fff0cc1f5</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -814,7 +814,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>54832180-8534-4b92-9a57-4176f97aacfa</t>
+          <t>78fef29f-aac1-48da-8b16-c80cb5477c44</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -860,7 +860,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>6c9080bb-8061-4711-b02a-7da01338beb8</t>
+          <t>30471ab7-ea71-480e-a311-459c261009c6</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -906,7 +906,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>c45d0f6d-e5c1-4d33-94f5-2e886b60bf19</t>
+          <t>d69af814-f329-4aa8-af85-42f1510c83c3</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -952,7 +952,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>10ffe120-07be-4ac0-a3ee-2417c74c09ad</t>
+          <t>66d9d4d1-2522-46ae-8e8c-74cf83b0c8a9</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4c42a4de-c483-4b00-9621-9bbfd1c3a6e5</t>
+          <t>0cf2d1a7-05a1-47da-b6fd-1d3d8e821560</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1044,7 +1044,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>4e2f94bd-6e7f-47c6-99ad-48b96ff1a18b</t>
+          <t>5cf5c49a-8520-4dc8-b6a5-615b23a4cd37</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1090,7 +1090,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>f5e1e006-f68b-4a12-a7ea-10f71a9f73a6</t>
+          <t>bc03209c-34a6-4ef6-8e16-c8dd11e91222</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1136,7 +1136,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>40c98c1d-9f79-456e-ae83-a5703fa69e74</t>
+          <t>6e29e66a-19b5-435f-86f1-621f4e1e2d90</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,19 +1170,19 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>da62cb63-8bf7-4b28-8536-bfa48dcdebb7</t>
+          <t>c86d904d-e99d-4a2c-b3b8-0a7633148ae1</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1228,7 +1228,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>78469df7-4600-4f34-a464-3abf5b3946b9</t>
+          <t>cce28004-92b0-486c-8e20-90e6607453bc</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1274,7 +1274,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>dd901bee-2756-43e2-b2b0-0dfca5c04baa</t>
+          <t>b72ae262-fded-42d8-8835-c03ab20883a9</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">

</xml_diff>

<commit_message>
teste aviso + 3 moscas
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafael/Desktop/git_hub/tese_public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E753D4-4659-1044-BDCD-F38AE62B91CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD7A701-11A5-2C4A-AE3D-10C9C59367B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4880" yWindow="500" windowWidth="46320" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -610,7 +610,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="184" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1243,7 +1243,7 @@
         <v>11</v>
       </c>
       <c r="C20" s="2">
-        <v>45862</v>
+        <v>45866</v>
       </c>
       <c r="D20" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-12 21:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,526</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-14 21:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-15 09:00:37
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-09-16 09:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807110716_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-16 21:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-17 09:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-09-18 09:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807110716_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-18 21:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-19 10:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-19 22:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,830,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-20 10:00:45
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,526</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-20 22:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-21 09:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807110716_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-09-21 21:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807110716_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,830,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-22 08:00:47
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,526</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-22 21:00:28
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-23 08:00:46
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807110716_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-09-23 09:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807110716_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,830,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-23 21:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,526</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-24 09:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-24 21:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-25 08:00:57
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-25 09:00:37
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-25 21:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-26 08:00:36
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-26 21:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-27 09:00:26
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-27 21:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-09-29 08:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-01 08:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-01 12:00:37
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-02 00:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-02 06:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-02 12:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808100711_ppp0.jpg</t>
+          <t>image_20250808221835_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,409,1232,451</t>
+          <t>1182,405,1231,455</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.75</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-03 13:00:28
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-03 18:00:28
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-04 00:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807110716_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,830,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-05 07:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,526</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-05 11:00:38
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-05 13:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-05 19:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111314_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>794,481,830,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-06 01:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111314_ppp0.jpg</t>
+          <t>image_20250807110716_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,526</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-06 14:00:38
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807110716_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-10-06 17:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-06 23:00:28
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-07 05:00:29
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807110716_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-10-07 11:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807110716_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-10-07 18:00:27
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807111728_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,830,525</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.70</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-08 09:00:37
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111728_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,12 +1124,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,830,525</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-08 17:00:39
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807111344_ppp0.jpg</t>
+          <t>image_20250807110716_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>794,481,831,526</t>
+          <t>793,481,831,527</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática: 2025-10-08 23:00:28
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807110716_ppp0.jpg</t>
+          <t>image_20250807110238_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>image_20250808221835_ppp0.jpg</t>
+          <t>image_20250808100711_ppp0.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1170,12 +1170,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1182,405,1231,455</t>
+          <t>1182,409,1232,451</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática: 2025-10-09 05:00:28
</commit_message>
<xml_diff>
--- a/dashboard_data.xlsx
+++ b/dashboard_data.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>image_20250807110238_ppp0.jpg</t>
+          <t>image_20250807111344_ppp0.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>793,481,831,527</t>
+          <t>794,481,831,526</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">

</xml_diff>